<commit_message>
Updated lot mapping files 2024-04-26
</commit_message>
<xml_diff>
--- a/gx_lotmapping/std_curve_params.xlsx
+++ b/gx_lotmapping/std_curve_params.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://022gc.sharepoint.com/sites/Communicablediseasesandinfectioncontrol-ScienceandTechnol426/Shared Documents/Wastewater/GX github files/gx_lotmapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8BF7DC56-FD1F-4741-AB42-BF515F82A17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:40009_{8BF7DC56-FD1F-4741-AB42-BF515F82A17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC6377E4-537A-484E-BD7C-3D3FD3A3FA7A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="std_curve_params" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="58">
   <si>
     <t>Cartridge Lot Number</t>
   </si>
@@ -199,7 +212,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -677,9 +690,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1034,11 +1050,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,7 +2007,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="2">
         <v>13816</v>
       </c>
       <c r="B48" t="s">
@@ -2011,7 +2027,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="2">
         <v>14018</v>
       </c>
       <c r="B49" t="s">
@@ -2031,7 +2047,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="2">
         <v>14019</v>
       </c>
       <c r="B50" t="s">
@@ -2051,7 +2067,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="2">
         <v>14714</v>
       </c>
       <c r="B51" t="s">
@@ -2071,7 +2087,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="2">
         <v>14903</v>
       </c>
       <c r="B52" t="s">
@@ -2091,7 +2107,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="2">
         <v>20201</v>
       </c>
       <c r="B53" t="s">
@@ -2111,7 +2127,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="2">
         <v>20204</v>
       </c>
       <c r="B54" t="s">
@@ -2131,7 +2147,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="2">
         <v>20205</v>
       </c>
       <c r="B55" t="s">
@@ -2151,7 +2167,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="2">
         <v>20206</v>
       </c>
       <c r="B56" t="s">
@@ -2171,7 +2187,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="2">
         <v>22920</v>
       </c>
       <c r="B57" t="s">
@@ -2191,7 +2207,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="2">
         <v>42514</v>
       </c>
       <c r="B58" t="s">
@@ -2211,7 +2227,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="2">
         <v>43109</v>
       </c>
       <c r="B59" t="s">
@@ -2227,6 +2243,26 @@
         <v>10</v>
       </c>
       <c r="F59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>43302</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2236,6 +2272,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ab521e1-8720-4533-8025-5c945dd49c24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC70BFA850CCAE47A7BAA0F38D9D36E7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ca04f000950caa8121282a10b5ee4284">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ab521e1-8720-4533-8025-5c945dd49c24" xmlns:ns3="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7a7c827840bdaa11f304efd419307b4" ns2:_="" ns3:_="">
     <xsd:import namespace="4ab521e1-8720-4533-8025-5c945dd49c24"/>
@@ -2464,34 +2520,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ab521e1-8720-4533-8025-5c945dd49c24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1557CBC2-664F-4BAE-96F8-E7372F324347}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3305E1E3-DAA1-4965-97DA-EEFD152C6338}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3305E1E3-DAA1-4965-97DA-EEFD152C6338}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBC8AA1D-4A1F-4E6B-AEE1-0D75C632111C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ab521e1-8720-4533-8025-5c945dd49c24"/>
+    <ds:schemaRef ds:uri="16e82f90-a588-4221-9ba0-cc9a2dc4dcab"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBC8AA1D-4A1F-4E6B-AEE1-0D75C632111C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1557CBC2-664F-4BAE-96F8-E7372F324347}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4ab521e1-8720-4533-8025-5c945dd49c24"/>
+    <ds:schemaRef ds:uri="16e82f90-a588-4221-9ba0-cc9a2dc4dcab"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated gx_lotmapping files to include 27720 and 49801 to use most recent std curves
</commit_message>
<xml_diff>
--- a/gx_lotmapping/std_curve_params.xlsx
+++ b/gx_lotmapping/std_curve_params.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://022gc.sharepoint.com/sites/Communicablediseasesandinfectioncontrol-ScienceandTechnol426/Shared Documents/Wastewater/GX github files/gx_lotmapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yjin\Documents\projects\GeneXpert_WW\gx_lotmapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:40009_{8BF7DC56-FD1F-4741-AB42-BF515F82A17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC6377E4-537A-484E-BD7C-3D3FD3A3FA7A}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200"/>
   </bookViews>
   <sheets>
     <sheet name="std_curve_params" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="58">
   <si>
     <t>Cartridge Lot Number</t>
   </si>
@@ -212,7 +211,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -690,11 +689,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1050,11 +1052,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,8 +2209,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>42514</v>
+      <c r="A58" s="3">
+        <v>27720</v>
       </c>
       <c r="B58" t="s">
         <v>26</v>
@@ -2227,8 +2229,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>43109</v>
+      <c r="A59" s="3">
+        <v>42514</v>
       </c>
       <c r="B59" t="s">
         <v>26</v>
@@ -2247,8 +2249,8 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>43302</v>
+      <c r="A60" s="3">
+        <v>43109</v>
       </c>
       <c r="B60" t="s">
         <v>26</v>
@@ -2263,6 +2265,66 @@
         <v>10</v>
       </c>
       <c r="F60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>43302</v>
+      </c>
+      <c r="B61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>48116</v>
+      </c>
+      <c r="B62" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>49801</v>
+      </c>
+      <c r="B63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2272,26 +2334,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ab521e1-8720-4533-8025-5c945dd49c24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC70BFA850CCAE47A7BAA0F38D9D36E7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ca04f000950caa8121282a10b5ee4284">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ab521e1-8720-4533-8025-5c945dd49c24" xmlns:ns3="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7a7c827840bdaa11f304efd419307b4" ns2:_="" ns3:_="">
     <xsd:import namespace="4ab521e1-8720-4533-8025-5c945dd49c24"/>
@@ -2520,10 +2562,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ab521e1-8720-4533-8025-5c945dd49c24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3305E1E3-DAA1-4965-97DA-EEFD152C6338}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1557CBC2-664F-4BAE-96F8-E7372F324347}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4ab521e1-8720-4533-8025-5c945dd49c24"/>
+    <ds:schemaRef ds:uri="16e82f90-a588-4221-9ba0-cc9a2dc4dcab"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2540,20 +2613,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1557CBC2-664F-4BAE-96F8-E7372F324347}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3305E1E3-DAA1-4965-97DA-EEFD152C6338}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4ab521e1-8720-4533-8025-5c945dd49c24"/>
-    <ds:schemaRef ds:uri="16e82f90-a588-4221-9ba0-cc9a2dc4dcab"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update GXWW_conversion and gx_lotmapping files to use most recent standard curves for lot 05608 ahead of new standard curve waiting approval
</commit_message>
<xml_diff>
--- a/gx_lotmapping/std_curve_params.xlsx
+++ b/gx_lotmapping/std_curve_params.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="std_curve_params" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="59">
   <si>
     <t>Cartridge Lot Number</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>07026</t>
+  </si>
+  <si>
+    <t>05608</t>
   </si>
 </sst>
 </file>
@@ -1053,22 +1056,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +1091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1108,7 +1111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1188,7 +1191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1308,7 +1311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1348,7 +1351,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1368,7 +1371,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1388,7 +1391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1428,7 +1431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1448,609 +1451,609 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B44" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" t="s">
-        <v>10</v>
-      </c>
-      <c r="F46" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>26</v>
       </c>
-      <c r="C47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
         <v>13816</v>
       </c>
-      <c r="B48" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
         <v>14018</v>
-      </c>
-      <c r="B49" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>14019</v>
       </c>
       <c r="B50" t="s">
         <v>26</v>
@@ -2068,9 +2071,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
-        <v>14714</v>
+        <v>14019</v>
       </c>
       <c r="B51" t="s">
         <v>26</v>
@@ -2088,49 +2091,49 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
+        <v>14714</v>
+      </c>
+      <c r="B52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
         <v>14903</v>
       </c>
-      <c r="B52" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
         <v>20201</v>
-      </c>
-      <c r="B53" t="s">
-        <v>26</v>
-      </c>
-      <c r="C53" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>20204</v>
       </c>
       <c r="B54" t="s">
         <v>26</v>
@@ -2148,9 +2151,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
-        <v>20205</v>
+        <v>20204</v>
       </c>
       <c r="B55" t="s">
         <v>26</v>
@@ -2168,9 +2171,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
-        <v>20206</v>
+        <v>20205</v>
       </c>
       <c r="B56" t="s">
         <v>26</v>
@@ -2188,9 +2191,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
-        <v>22920</v>
+        <v>20206</v>
       </c>
       <c r="B57" t="s">
         <v>26</v>
@@ -2208,9 +2211,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
-        <v>27720</v>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>22920</v>
       </c>
       <c r="B58" t="s">
         <v>26</v>
@@ -2228,9 +2231,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
-        <v>42514</v>
+        <v>27720</v>
       </c>
       <c r="B59" t="s">
         <v>26</v>
@@ -2248,9 +2251,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
-        <v>43109</v>
+        <v>42514</v>
       </c>
       <c r="B60" t="s">
         <v>26</v>
@@ -2268,9 +2271,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
-        <v>43302</v>
+        <v>43109</v>
       </c>
       <c r="B61" t="s">
         <v>26</v>
@@ -2288,9 +2291,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
-        <v>48116</v>
+        <v>43302</v>
       </c>
       <c r="B62" t="s">
         <v>26</v>
@@ -2308,9 +2311,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <v>49801</v>
+        <v>48116</v>
       </c>
       <c r="B63" t="s">
         <v>26</v>
@@ -2325,6 +2328,26 @@
         <v>10</v>
       </c>
       <c r="F63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
+        <v>49801</v>
+      </c>
+      <c r="B64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2334,6 +2357,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ab521e1-8720-4533-8025-5c945dd49c24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC70BFA850CCAE47A7BAA0F38D9D36E7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ca04f000950caa8121282a10b5ee4284">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ab521e1-8720-4533-8025-5c945dd49c24" xmlns:ns3="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7a7c827840bdaa11f304efd419307b4" ns2:_="" ns3:_="">
     <xsd:import namespace="4ab521e1-8720-4533-8025-5c945dd49c24"/>
@@ -2562,27 +2605,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ab521e1-8720-4533-8025-5c945dd49c24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="16e82f90-a588-4221-9ba0-cc9a2dc4dcab" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBC8AA1D-4A1F-4E6B-AEE1-0D75C632111C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ab521e1-8720-4533-8025-5c945dd49c24"/>
+    <ds:schemaRef ds:uri="16e82f90-a588-4221-9ba0-cc9a2dc4dcab"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3305E1E3-DAA1-4965-97DA-EEFD152C6338}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1557CBC2-664F-4BAE-96F8-E7372F324347}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2599,23 +2641,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBC8AA1D-4A1F-4E6B-AEE1-0D75C632111C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ab521e1-8720-4533-8025-5c945dd49c24"/>
-    <ds:schemaRef ds:uri="16e82f90-a588-4221-9ba0-cc9a2dc4dcab"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3305E1E3-DAA1-4965-97DA-EEFD152C6338}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>